<commit_message>
selecionando data venda, tem que criar para salvar relatorio
</commit_message>
<xml_diff>
--- a/public/relatorio_vendas.xlsx
+++ b/public/relatorio_vendas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Cliente</t>
   </si>
@@ -36,36 +36,21 @@
     <t>Data</t>
   </si>
   <si>
-    <t>LEONARDO/ Responsavel Iranildo 2</t>
+    <t>Cliente Porta</t>
   </si>
   <si>
     <t>Cimento Nassau 50kg</t>
   </si>
   <si>
-    <t>cartão 2x</t>
+    <t>A Vista - Pix</t>
+  </si>
+  <si>
+    <t>27/04/2023</t>
   </si>
   <si>
     <t>26/04/2023</t>
   </si>
   <si>
-    <t>pix</t>
-  </si>
-  <si>
-    <t>Cliente Porta</t>
-  </si>
-  <si>
-    <t>A Vista - Pix</t>
-  </si>
-  <si>
-    <t>27/04/2023</t>
-  </si>
-  <si>
-    <t>28/04/2023</t>
-  </si>
-  <si>
-    <t>29/05/2023</t>
-  </si>
-  <si>
     <t>Diaria</t>
   </si>
   <si>
@@ -78,7 +63,7 @@
     <t>MÊS REFERÊNCIA</t>
   </si>
   <si>
-    <t>05</t>
+    <t>04</t>
   </si>
 </sst>
 </file>
@@ -418,7 +403,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,10 +439,10 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>70.0</v>
+        <v>35.0</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -474,96 +459,16 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>175.0</v>
+        <v>70.0</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>175.0</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>189.95</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>35.99</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>71.98</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -597,30 +502,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>297.92</v>
+        <v>105.0</v>
       </c>
       <c r="B2">
-        <v>717.92</v>
+        <v>105.0</v>
       </c>
       <c r="C2">
-        <v>717.92</v>
+        <v>105.0</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criando jobs, funcionando com dados aleatorios
</commit_message>
<xml_diff>
--- a/public/relatorio_vendas.xlsx
+++ b/public/relatorio_vendas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Cliente</t>
   </si>
@@ -33,22 +33,28 @@
     <t>Pagamentos</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Cliente Porta</t>
-  </si>
-  <si>
-    <t>Cimento Nassau 50kg</t>
-  </si>
-  <si>
-    <t>A Vista - Pix</t>
-  </si>
-  <si>
-    <t>27/04/2023</t>
-  </si>
-  <si>
-    <t>26/04/2023</t>
+    <t>Data Venda</t>
+  </si>
+  <si>
+    <t>devic</t>
+  </si>
+  <si>
+    <t>Cimento nassau</t>
+  </si>
+  <si>
+    <t>pix</t>
+  </si>
+  <si>
+    <t>21/03/2023</t>
+  </si>
+  <si>
+    <t>23/01/2023</t>
+  </si>
+  <si>
+    <t>28/03/2023</t>
+  </si>
+  <si>
+    <t>29/04/2023</t>
   </si>
   <si>
     <t>Diaria</t>
@@ -403,7 +409,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,10 +445,10 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>35.0</v>
+        <v>925.0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -459,16 +465,56 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>70.0</v>
+        <v>23.0</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>70.0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>35.0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -502,30 +548,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>105.0</v>
+        <v>35.0</v>
       </c>
       <c r="B2">
-        <v>105.0</v>
+        <v>1053.0</v>
       </c>
       <c r="C2">
-        <v>105.0</v>
+        <v>1053.0</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcao relatorio no dashboard
</commit_message>
<xml_diff>
--- a/public/relatorio_vendas.xlsx
+++ b/public/relatorio_vendas.xlsx
@@ -7,7 +7,9 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Vendas" sheetId="1" r:id="rId4"/>
+    <sheet name="Março" sheetId="1" r:id="rId4"/>
+    <sheet name="Janeiro" sheetId="2" r:id="rId5"/>
+    <sheet name="Abril" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -15,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Cliente</t>
   </si>
@@ -35,9 +37,6 @@
     <t>Dia Venda</t>
   </si>
   <si>
-    <t>Mes Venda</t>
-  </si>
-  <si>
     <t>devic</t>
   </si>
   <si>
@@ -45,15 +44,6 @@
   </si>
   <si>
     <t>pix</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>04</t>
   </si>
 </sst>
 </file>
@@ -393,7 +383,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -401,7 +391,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,16 +410,13 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2">
         <v>925.0</v>
@@ -438,82 +425,168 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3">
+        <v>70.0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="F3">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>23.0</v>
       </c>
-      <c r="D3">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C2">
+        <v>35.0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>70.0</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>35.0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5">
+      <c r="F2">
         <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionado edicao de cliente
</commit_message>
<xml_diff>
--- a/public/relatorio_vendas.xlsx
+++ b/public/relatorio_vendas.xlsx
@@ -4,16 +4,55 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="-1" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
-  <sheets/>
+  <sheets>
+    <sheet name="Maio" sheetId="1" r:id="rId4"/>
+  </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Valor da venda</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Pagamentos</t>
+  </si>
+  <si>
+    <t>Dia Venda</t>
+  </si>
+  <si>
+    <t>Cliente Porta</t>
+  </si>
+  <si>
+    <t>Cimento Nassau 50kg</t>
+  </si>
+  <si>
+    <t>espécie</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>A Vista - Pix</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -344,4 +383,113 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>35.0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>175.0</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1725.0</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
 </file>
</xml_diff>